<commit_message>
Update Realisasi TUP Tahap 2 dan GUP Nihil
</commit_message>
<xml_diff>
--- a/REALISASI PUSDIK/Justifikasi Sisa Anggaran yang tidak terserap.xlsx
+++ b/REALISASI PUSDIK/Justifikasi Sisa Anggaran yang tidak terserap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BACK\PUSDIK\2022\Realisasi\ArifMustaqim\TA.2022\REALISASI PUSDIK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57FEC2F7-7268-4CD3-85BE-CF71E1A77CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B654393-3CD3-4403-B181-91CAD8A46B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{268D5237-A487-409D-A0BE-AE0394B6CC03}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Justifikasi!$A$3:$E$40</definedName>
     <definedName name="Belanja_Perjalanan_Dinas_Paket_Meeting_Dalam_Kota._Uang_Saku_RDK_dalam__Verifikasi_dan_Pembuatan_Format_Standart_Data_BKU_Satker_Pusat_Pendidikan_KP___tgl.__27__Februari__2020">#REF!</definedName>
     <definedName name="cAkun">#REF!</definedName>
-    <definedName name="Cetak_dinamis">OFFSET('[2]DASHBOARD SP2D'!$B$1,0,0,COUNTA('[2]DASHBOARD SP2D'!$G:$G),6)</definedName>
+    <definedName name="Cetak_dinamis">OFFSET('[1]DASHBOARD SP2D'!$B$1,0,0,COUNTA('[1]DASHBOARD SP2D'!$G:$G),6)</definedName>
     <definedName name="chkAkun">#REF!</definedName>
     <definedName name="chkKegiatan">#REF!</definedName>
     <definedName name="chkKomponen">#REF!</definedName>
@@ -42,21 +42,21 @@
     <definedName name="Entri_Es2">#REF!</definedName>
     <definedName name="Entri_Es3">#REF!</definedName>
     <definedName name="Entri_Es4">#REF!</definedName>
-    <definedName name="Eselon3">[3]eselon3_4!$A$2:$A$7</definedName>
-    <definedName name="Eselon4">[3]eselon3_4!$B$2:$B$11</definedName>
-    <definedName name="FILTER_LAP">'[2]DASHBOARD SP2D'!#REF!</definedName>
+    <definedName name="Eselon3">[2]eselon3_4!$A$2:$A$7</definedName>
+    <definedName name="Eselon4">[2]eselon3_4!$B$2:$B$11</definedName>
+    <definedName name="FILTER_LAP">'[1]DASHBOARD SP2D'!#REF!</definedName>
     <definedName name="kegiatan">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Justifikasi!$A$1:$E$44</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Justifikasi!$3:$3</definedName>
-    <definedName name="rngSP2D">'[4]Tambahan Realisasi'!$C$2</definedName>
+    <definedName name="rngSP2D">'[3]Tambahan Realisasi'!$C$2</definedName>
     <definedName name="rowEselon2">#REF!</definedName>
     <definedName name="rowKoord">#REF!</definedName>
     <definedName name="rowSelect">#REF!</definedName>
     <definedName name="rowSubKoord">#REF!</definedName>
-    <definedName name="SSBP">[2]SSBP!#REF!</definedName>
+    <definedName name="SSBP">[1]SSBP!#REF!</definedName>
     <definedName name="Start_Jadi">#REF!</definedName>
-    <definedName name="TGL_SP2D">[2]DASHBOARD!$I$1</definedName>
-    <definedName name="TglRealisasi">'[1]Setting Database'!$B$12</definedName>
+    <definedName name="TGL_SP2D">[1]DASHBOARD!$I$1</definedName>
+    <definedName name="TglRealisasi">'[4]Setting Database'!$B$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -390,9 +390,6 @@
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,9 +409,6 @@
     <xf numFmtId="41" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -426,9 +420,6 @@
     </xf>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -493,14 +484,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="41" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -525,147 +525,6 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="DIPA4_PUSDIK (2)"/>
-      <sheetName val="Setting Database"/>
-      <sheetName val="Estimasi Presisi Realisasi"/>
-      <sheetName val="DIPA Rev 7"/>
-      <sheetName val="Sheet5"/>
-      <sheetName val="DIPA Revisi 3"/>
-      <sheetName val="Realisasi Pusdik Versi Ses"/>
-      <sheetName val="Semula Menjadi"/>
-      <sheetName val="DIPA Rev 7 Plus Gaji"/>
-      <sheetName val="Rencana GUP dan LS"/>
-      <sheetName val="SP2D ON"/>
-      <sheetName val="Pagu Per Jenis Akun2"/>
-      <sheetName val="PERAKUN"/>
-      <sheetName val="GUP TUP"/>
-      <sheetName val="SP2D"/>
-      <sheetName val="PivotSP2D"/>
-      <sheetName val="Matrik Percepatan Realisasi"/>
-      <sheetName val="Laporan ke KABAG"/>
-      <sheetName val="Lap FA Detil + Gaji"/>
-      <sheetName val="Sisa SP2D + Fisik"/>
-      <sheetName val="Pagu dan Sisa SP2D"/>
-      <sheetName val="Sisa Per Status Akun"/>
-      <sheetName val="Sisa Per Bidang"/>
-      <sheetName val="Laporan Per Akun + Fisik"/>
-      <sheetName val="Laporan Fisik"/>
-      <sheetName val="SPP LS"/>
-      <sheetName val="Sheet6"/>
-      <sheetName val="SP2D_NEW"/>
-      <sheetName val="SPAN vs SAKTI (Tanpa Gaji)"/>
-      <sheetName val="SPAN vs SAKTI (Plus Gaji)"/>
-      <sheetName val="Proyeksi des (non Gaji)"/>
-      <sheetName val="Proyeksi des (Plus Gaji)"/>
-      <sheetName val="Laporan Per Akun (2)"/>
-      <sheetName val="Rencana Realisasi"/>
-      <sheetName val="Laporan Per Akun"/>
-      <sheetName val="Buat Evaluasi"/>
-      <sheetName val="Sheet4"/>
-      <sheetName val="SP2D_New Per Bulan"/>
-      <sheetName val="Realisasi Per Bulan"/>
-      <sheetName val="Pivot SPP"/>
-      <sheetName val="Lampiran SPP"/>
-      <sheetName val="SP2D OMSPAN"/>
-      <sheetName val="Sheet3"/>
-      <sheetName val="DBSPBY"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet7"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="MonSPPSPMSP2D"/>
-      <sheetName val="Target"/>
-      <sheetName val="Hal3DIPA"/>
-      <sheetName val="SAKTI-Monitoring SPP"/>
-      <sheetName val="Arsip SPP"/>
-      <sheetName val="Sheet9"/>
-      <sheetName val="pvtKarwas"/>
-      <sheetName val="Karwas"/>
-      <sheetName val="Sheet8"/>
-      <sheetName val="SP2D Gaji"/>
-      <sheetName val="PER BULAN"/>
-      <sheetName val="Real SPAN vs SAKTI (Tanpa Gaji)"/>
-      <sheetName val="Real SPAN vs SAKTI (Plus Gaji)"/>
-      <sheetName val="DIPA3"/>
-      <sheetName val="HistoryDIPA"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="12">
-          <cell r="B12" t="str">
-            <v>26 DESEMBER 2022</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2694,7 +2553,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2832,7 +2691,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2958,6 +2817,147 @@
       <sheetData sheetId="54" refreshError="1"/>
       <sheetData sheetId="55" refreshError="1"/>
       <sheetData sheetId="56" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="DIPA4_PUSDIK (2)"/>
+      <sheetName val="Setting Database"/>
+      <sheetName val="Estimasi Presisi Realisasi"/>
+      <sheetName val="DIPA Rev 7"/>
+      <sheetName val="Justifikasi yg tdk terserap"/>
+      <sheetName val="DIPA Revisi 3"/>
+      <sheetName val="Realisasi Pusdik Versi Ses"/>
+      <sheetName val="Semula Menjadi"/>
+      <sheetName val="DIPA Rev 7 Plus Gaji"/>
+      <sheetName val="Rencana GUP dan LS"/>
+      <sheetName val="SP2D ON"/>
+      <sheetName val="Pagu Per Jenis Akun2"/>
+      <sheetName val="PERAKUN"/>
+      <sheetName val="GUP TUP"/>
+      <sheetName val="SP2D"/>
+      <sheetName val="PivotSP2D"/>
+      <sheetName val="Matrik Percepatan Realisasi"/>
+      <sheetName val="Laporan ke KABAG"/>
+      <sheetName val="Lap FA Detil + Gaji"/>
+      <sheetName val="Sisa SP2D + Fisik"/>
+      <sheetName val="Pagu dan Sisa SP2D"/>
+      <sheetName val="Sisa Per Status Akun"/>
+      <sheetName val="Sisa Per Bidang"/>
+      <sheetName val="Laporan Per Akun + Fisik"/>
+      <sheetName val="Laporan Fisik"/>
+      <sheetName val="SPP LS"/>
+      <sheetName val="Sheet6"/>
+      <sheetName val="SP2D_NEW"/>
+      <sheetName val="SPAN vs SAKTI (Tanpa Gaji)"/>
+      <sheetName val="SPAN vs SAKTI (Plus Gaji)"/>
+      <sheetName val="Proyeksi des (non Gaji)"/>
+      <sheetName val="Proyeksi des (Plus Gaji)"/>
+      <sheetName val="Laporan Per Akun (2)"/>
+      <sheetName val="Rencana Realisasi"/>
+      <sheetName val="Laporan Per Akun"/>
+      <sheetName val="Buat Evaluasi"/>
+      <sheetName val="Sheet4"/>
+      <sheetName val="SP2D_New Per Bulan"/>
+      <sheetName val="Realisasi Per Bulan"/>
+      <sheetName val="Pivot SPP"/>
+      <sheetName val="Lampiran SPP"/>
+      <sheetName val="SP2D OMSPAN"/>
+      <sheetName val="Sheet3"/>
+      <sheetName val="DBSPBY"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet7"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="MonSPPSPMSP2D"/>
+      <sheetName val="Target"/>
+      <sheetName val="Hal3DIPA"/>
+      <sheetName val="SAKTI-Monitoring SPP"/>
+      <sheetName val="Arsip SPP"/>
+      <sheetName val="Sheet9"/>
+      <sheetName val="pvtKarwas"/>
+      <sheetName val="Karwas"/>
+      <sheetName val="Sheet8"/>
+      <sheetName val="SP2D Gaji"/>
+      <sheetName val="PER BULAN"/>
+      <sheetName val="Real SPAN vs SAKTI (Tanpa Gaji)"/>
+      <sheetName val="Real SPAN vs SAKTI (Plus Gaji)"/>
+      <sheetName val="DIPA3"/>
+      <sheetName val="HistoryDIPA"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="12">
+          <cell r="B12" t="str">
+            <v>26 DESEMBER 2022</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="57" refreshError="1"/>
+      <sheetData sheetId="58" refreshError="1"/>
+      <sheetData sheetId="59" refreshError="1"/>
+      <sheetData sheetId="60" refreshError="1"/>
+      <sheetData sheetId="61" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3265,470 +3265,470 @@
   </sheetPr>
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="35"/>
-    <col min="2" max="2" width="30.109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" style="39" customWidth="1"/>
-    <col min="5" max="5" width="46" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="32"/>
+    <col min="2" max="2" width="30.109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="35" customWidth="1"/>
+    <col min="5" max="5" width="46" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="10" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+    <row r="4" spans="1:5" s="8" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>2010000</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="10" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12" t="s">
+    <row r="5" spans="1:5" s="8" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="11">
         <v>2010000</v>
       </c>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="6" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="E5" s="39"/>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>10479950</v>
       </c>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="1:5" s="10" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="12" t="s">
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="11">
         <v>10479950</v>
       </c>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="7" t="s">
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>11501820</v>
       </c>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" spans="1:5" s="10" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="12" t="s">
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="11">
         <v>3600000</v>
       </c>
-      <c r="E9" s="18"/>
-    </row>
-    <row r="10" spans="1:5" s="10" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="12" t="s">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:5" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="11">
         <v>7901820</v>
       </c>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
         <v>3</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <v>3600000</v>
       </c>
-      <c r="E11" s="15"/>
-    </row>
-    <row r="12" spans="1:5" s="10" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="12" t="s">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="11">
         <v>3600000</v>
       </c>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="7" t="s">
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>103093869</v>
       </c>
-      <c r="E13" s="19"/>
-    </row>
-    <row r="14" spans="1:5" s="10" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="20" t="s">
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:5" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="18">
         <v>4600150</v>
       </c>
-      <c r="E14" s="22"/>
-    </row>
-    <row r="15" spans="1:5" s="10" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="20" t="s">
+      <c r="E14" s="19"/>
+    </row>
+    <row r="15" spans="1:5" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="18">
         <v>77068149</v>
       </c>
-      <c r="E15" s="22"/>
-    </row>
-    <row r="16" spans="1:5" s="10" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="20" t="s">
+      <c r="E15" s="19"/>
+    </row>
+    <row r="16" spans="1:5" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="18">
         <v>2750120</v>
       </c>
-      <c r="E16" s="22"/>
-    </row>
-    <row r="17" spans="1:5" s="10" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="20" t="s">
+      <c r="E16" s="19"/>
+    </row>
+    <row r="17" spans="1:5" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="18">
         <v>8160450</v>
       </c>
-      <c r="E17" s="22"/>
-    </row>
-    <row r="18" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="23" t="s">
+      <c r="E17" s="19"/>
+    </row>
+    <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
-    </row>
-    <row r="19" spans="1:5" s="10" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="24" t="s">
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+    </row>
+    <row r="19" spans="1:5" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="18">
         <v>2265000</v>
       </c>
-      <c r="E19" s="22"/>
-    </row>
-    <row r="20" spans="1:5" s="10" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="24" t="s">
+      <c r="E19" s="19"/>
+    </row>
+    <row r="20" spans="1:5" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="18">
         <v>8250000</v>
       </c>
-      <c r="E20" s="25"/>
+      <c r="E20" s="22"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26" t="s">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="28">
+      <c r="D21" s="25">
         <v>281806436</v>
       </c>
-      <c r="E21" s="19"/>
+      <c r="E21" s="16"/>
     </row>
     <row r="22" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="20" t="s">
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="18">
         <v>151619602</v>
       </c>
-      <c r="E22" s="22"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="20" t="s">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="18">
         <v>9800000</v>
       </c>
-      <c r="E23" s="22"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="20" t="s">
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="18">
         <v>2155654</v>
       </c>
-      <c r="E24" s="22"/>
+      <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="23" t="s">
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="22"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="29" t="s">
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="18">
         <v>13050000</v>
       </c>
-      <c r="E26" s="22"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="29" t="s">
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="21">
+      <c r="D27" s="18">
         <v>26250000</v>
       </c>
-      <c r="E27" s="22"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="29" t="s">
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="21">
+      <c r="D28" s="18">
         <v>63469180</v>
       </c>
-      <c r="E28" s="22"/>
+      <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="30" t="s">
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="31"/>
-      <c r="E29" s="22"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="24" t="s">
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="21">
+      <c r="D30" s="18">
         <v>6290000</v>
       </c>
-      <c r="E30" s="22"/>
+      <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="24" t="s">
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31" s="18">
         <v>9172000</v>
       </c>
-      <c r="E31" s="25"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="7" t="s">
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D32" s="29">
         <v>162041000</v>
       </c>
-      <c r="E32" s="19"/>
+      <c r="E32" s="16"/>
     </row>
     <row r="33" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="20" t="s">
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33" s="18">
         <v>20000000</v>
       </c>
-      <c r="E33" s="22"/>
+      <c r="E33" s="19"/>
     </row>
     <row r="34" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="20" t="s">
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="18">
         <v>142041000</v>
       </c>
-      <c r="E34" s="25"/>
+      <c r="E34" s="22"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="7" t="s">
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="32">
+      <c r="D35" s="29">
         <v>21925000</v>
       </c>
-      <c r="E35" s="19"/>
+      <c r="E35" s="16"/>
     </row>
     <row r="36" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="20" t="s">
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="18">
         <v>5965000</v>
       </c>
-      <c r="E36" s="22"/>
+      <c r="E36" s="19"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="33" t="s">
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="22"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="19"/>
     </row>
     <row r="38" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="24" t="s">
+      <c r="A38" s="23"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="21">
+      <c r="D38" s="18">
         <v>6180000</v>
       </c>
-      <c r="E38" s="22"/>
+      <c r="E38" s="19"/>
     </row>
     <row r="39" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="24" t="s">
+      <c r="A39" s="31"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="21">
+      <c r="D39" s="18">
         <v>9780000</v>
       </c>
-      <c r="E39" s="25"/>
+      <c r="E39" s="22"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="36"/>
-      <c r="D40" s="37">
+      <c r="C40" s="40"/>
+      <c r="D40" s="33">
         <f>SUM(D4,D6,D8,D11,D13,D21,D32,D35)</f>
         <v>596458075</v>
       </c>
-      <c r="E40" s="38"/>
+      <c r="E40" s="34"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="36" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>